<commit_message>
update disruptor system doc
</commit_message>
<xml_diff>
--- a/game/机型编年史.xlsx
+++ b/game/机型编年史.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="432">
   <si>
     <t>厂商</t>
   </si>
@@ -729,6 +729,12 @@
     <t>Nintendo</t>
   </si>
   <si>
+    <t>超级马里奥兄弟2</t>
+  </si>
+  <si>
+    <t>超级马里奥兄弟3</t>
+  </si>
+  <si>
     <t>双截龙1</t>
   </si>
   <si>
@@ -1334,10 +1340,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1355,9 +1361,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1365,6 +1370,52 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1393,37 +1444,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1434,6 +1463,22 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1454,45 +1499,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -1507,7 +1513,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1519,163 +1675,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1703,20 +1709,54 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1736,32 +1776,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1774,30 +1804,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1806,10 +1812,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1818,133 +1824,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3801,10 +3807,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F228"/>
+  <dimension ref="A1:F230"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -3859,7 +3865,7 @@
         <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D3">
         <v>1988</v>
@@ -3873,13 +3879,13 @@
     </row>
     <row r="4" spans="2:6">
       <c r="B4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C4" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D4">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -3890,13 +3896,13 @@
     </row>
     <row r="5" spans="2:6">
       <c r="B5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C5" t="s">
         <v>233</v>
       </c>
       <c r="D5">
-        <v>1990</v>
+        <v>1988</v>
       </c>
       <c r="E5" t="s">
         <v>11</v>
@@ -3907,13 +3913,13 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" t="s">
         <v>235</v>
       </c>
-      <c r="C6" t="s">
-        <v>229</v>
-      </c>
       <c r="D6">
-        <v>1981</v>
+        <v>1989</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
@@ -3927,10 +3933,10 @@
         <v>236</v>
       </c>
       <c r="C7" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="D7">
-        <v>1982</v>
+        <v>1990</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
@@ -3947,7 +3953,7 @@
         <v>229</v>
       </c>
       <c r="D8">
-        <v>1984</v>
+        <v>1981</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
@@ -3964,7 +3970,7 @@
         <v>229</v>
       </c>
       <c r="D9">
-        <v>1984</v>
+        <v>1982</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
@@ -3975,13 +3981,13 @@
     </row>
     <row r="10" spans="2:6">
       <c r="B10" t="s">
-        <v>125</v>
+        <v>239</v>
       </c>
       <c r="C10" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="D10">
-        <v>1990</v>
+        <v>1984</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -3992,30 +3998,30 @@
     </row>
     <row r="11" spans="2:6">
       <c r="B11" t="s">
-        <v>125</v>
+        <v>240</v>
       </c>
       <c r="C11" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="D11">
-        <v>1993</v>
+        <v>1984</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>241</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" t="s">
-        <v>242</v>
+        <v>125</v>
       </c>
       <c r="C12" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="D12">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -4026,19 +4032,19 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" t="s">
+        <v>242</v>
+      </c>
+      <c r="D13">
+        <v>1993</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="s">
         <v>243</v>
-      </c>
-      <c r="C13" t="s">
-        <v>240</v>
-      </c>
-      <c r="D13">
-        <v>1992</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="14" spans="2:6">
@@ -4046,10 +4052,10 @@
         <v>244</v>
       </c>
       <c r="C14" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="D14">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
@@ -4063,10 +4069,10 @@
         <v>245</v>
       </c>
       <c r="C15" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D15">
-        <v>1988</v>
+        <v>1992</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -4077,13 +4083,13 @@
     </row>
     <row r="16" spans="2:6">
       <c r="B16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C16" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D16">
-        <v>1990</v>
+        <v>1993</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
@@ -4094,13 +4100,13 @@
     </row>
     <row r="17" spans="2:6">
       <c r="B17" t="s">
+        <v>247</v>
+      </c>
+      <c r="C17" t="s">
         <v>248</v>
       </c>
-      <c r="C17" t="s">
-        <v>246</v>
-      </c>
       <c r="D17">
-        <v>1991</v>
+        <v>1988</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -4113,6 +4119,12 @@
       <c r="B18" t="s">
         <v>249</v>
       </c>
+      <c r="C18" t="s">
+        <v>248</v>
+      </c>
+      <c r="D18">
+        <v>1990</v>
+      </c>
       <c r="E18" t="s">
         <v>11</v>
       </c>
@@ -4125,10 +4137,10 @@
         <v>250</v>
       </c>
       <c r="C19" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D19">
-        <v>1987</v>
+        <v>1991</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -4139,13 +4151,7 @@
     </row>
     <row r="20" spans="2:6">
       <c r="B20" t="s">
-        <v>252</v>
-      </c>
-      <c r="C20" t="s">
-        <v>240</v>
-      </c>
-      <c r="D20">
-        <v>1993</v>
+        <v>251</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
@@ -4156,7 +4162,13 @@
     </row>
     <row r="21" spans="2:6">
       <c r="B21" t="s">
+        <v>252</v>
+      </c>
+      <c r="C21" t="s">
         <v>253</v>
+      </c>
+      <c r="D21">
+        <v>1987</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -4169,6 +4181,12 @@
       <c r="B22" t="s">
         <v>254</v>
       </c>
+      <c r="C22" t="s">
+        <v>242</v>
+      </c>
+      <c r="D22">
+        <v>1993</v>
+      </c>
       <c r="E22" t="s">
         <v>11</v>
       </c>
@@ -4191,9 +4209,6 @@
       <c r="B24" t="s">
         <v>256</v>
       </c>
-      <c r="D24">
-        <v>1994</v>
-      </c>
       <c r="E24" t="s">
         <v>11</v>
       </c>
@@ -4216,6 +4231,9 @@
       <c r="B26" t="s">
         <v>258</v>
       </c>
+      <c r="D26">
+        <v>1994</v>
+      </c>
       <c r="E26" t="s">
         <v>11</v>
       </c>
@@ -4260,12 +4278,6 @@
       <c r="B30" t="s">
         <v>262</v>
       </c>
-      <c r="C30" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30">
-        <v>1980</v>
-      </c>
       <c r="E30" t="s">
         <v>11</v>
       </c>
@@ -4273,48 +4285,48 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:6">
       <c r="B31" t="s">
         <v>263</v>
       </c>
-      <c r="C31" t="s">
-        <v>264</v>
-      </c>
-      <c r="D31">
-        <v>1990</v>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" t="s">
+        <v>264</v>
+      </c>
+      <c r="C32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D32">
+        <v>1980</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" t="s">
         <v>265</v>
       </c>
-      <c r="E32" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6">
-      <c r="B33" t="s">
-        <v>152</v>
-      </c>
       <c r="C33" t="s">
-        <v>240</v>
+        <v>266</v>
       </c>
       <c r="D33">
         <v>1990</v>
       </c>
-      <c r="E33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E34" t="s">
         <v>11</v>
@@ -4325,7 +4337,13 @@
     </row>
     <row r="35" spans="2:6">
       <c r="B35" t="s">
-        <v>267</v>
+        <v>152</v>
+      </c>
+      <c r="C35" t="s">
+        <v>242</v>
+      </c>
+      <c r="D35">
+        <v>1990</v>
       </c>
       <c r="E35" t="s">
         <v>11</v>
@@ -4437,9 +4455,6 @@
       <c r="B45" t="s">
         <v>277</v>
       </c>
-      <c r="C45" t="s">
-        <v>278</v>
-      </c>
       <c r="E45" t="s">
         <v>11</v>
       </c>
@@ -4449,9 +4464,6 @@
     </row>
     <row r="46" spans="2:6">
       <c r="B46" t="s">
-        <v>279</v>
-      </c>
-      <c r="C46" t="s">
         <v>278</v>
       </c>
       <c r="E46" t="s">
@@ -4463,10 +4475,10 @@
     </row>
     <row r="47" spans="2:6">
       <c r="B47" t="s">
+        <v>279</v>
+      </c>
+      <c r="C47" t="s">
         <v>280</v>
-      </c>
-      <c r="C47" t="s">
-        <v>278</v>
       </c>
       <c r="E47" t="s">
         <v>11</v>
@@ -4480,10 +4492,7 @@
         <v>281</v>
       </c>
       <c r="C48" t="s">
-        <v>278</v>
-      </c>
-      <c r="D48">
-        <v>1994</v>
+        <v>280</v>
       </c>
       <c r="E48" t="s">
         <v>11</v>
@@ -4496,6 +4505,9 @@
       <c r="B49" t="s">
         <v>282</v>
       </c>
+      <c r="C49" t="s">
+        <v>280</v>
+      </c>
       <c r="E49" t="s">
         <v>11</v>
       </c>
@@ -4507,6 +4519,12 @@
       <c r="B50" t="s">
         <v>283</v>
       </c>
+      <c r="C50" t="s">
+        <v>280</v>
+      </c>
+      <c r="D50">
+        <v>1994</v>
+      </c>
       <c r="E50" t="s">
         <v>11</v>
       </c>
@@ -4571,7 +4589,7 @@
     </row>
     <row r="56" spans="2:6">
       <c r="B56" t="s">
-        <v>204</v>
+        <v>289</v>
       </c>
       <c r="E56" t="s">
         <v>11</v>
@@ -4582,7 +4600,7 @@
     </row>
     <row r="57" spans="2:6">
       <c r="B57" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E57" t="s">
         <v>11</v>
@@ -4593,7 +4611,7 @@
     </row>
     <row r="58" spans="2:6">
       <c r="B58" t="s">
-        <v>290</v>
+        <v>204</v>
       </c>
       <c r="E58" t="s">
         <v>11</v>
@@ -4613,7 +4631,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="60" customFormat="1" spans="2:6">
+    <row r="60" spans="2:6">
       <c r="B60" t="s">
         <v>292</v>
       </c>
@@ -4635,7 +4653,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="62" spans="2:6">
+    <row r="62" customFormat="1" spans="2:6">
       <c r="B62" t="s">
         <v>294</v>
       </c>
@@ -4780,13 +4798,7 @@
     </row>
     <row r="75" spans="2:6">
       <c r="B75" t="s">
-        <v>166</v>
-      </c>
-      <c r="C75" t="s">
-        <v>278</v>
-      </c>
-      <c r="D75">
-        <v>1985</v>
+        <v>307</v>
       </c>
       <c r="E75" t="s">
         <v>11</v>
@@ -4797,7 +4809,7 @@
     </row>
     <row r="76" spans="2:6">
       <c r="B76" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E76" t="s">
         <v>11</v>
@@ -4808,7 +4820,13 @@
     </row>
     <row r="77" spans="2:6">
       <c r="B77" t="s">
-        <v>308</v>
+        <v>166</v>
+      </c>
+      <c r="C77" t="s">
+        <v>280</v>
+      </c>
+      <c r="D77">
+        <v>1985</v>
       </c>
       <c r="E77" t="s">
         <v>11</v>
@@ -4918,7 +4936,7 @@
     </row>
     <row r="87" spans="2:6">
       <c r="B87" t="s">
-        <v>287</v>
+        <v>318</v>
       </c>
       <c r="E87" t="s">
         <v>11</v>
@@ -4929,7 +4947,7 @@
     </row>
     <row r="88" spans="2:6">
       <c r="B88" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E88" t="s">
         <v>11</v>
@@ -4940,7 +4958,7 @@
     </row>
     <row r="89" spans="2:6">
       <c r="B89" t="s">
-        <v>319</v>
+        <v>289</v>
       </c>
       <c r="E89" t="s">
         <v>11</v>
@@ -4950,14 +4968,8 @@
       </c>
     </row>
     <row r="90" spans="2:6">
-      <c r="B90" s="3" t="s">
+      <c r="B90" t="s">
         <v>320</v>
-      </c>
-      <c r="C90" t="s">
-        <v>240</v>
-      </c>
-      <c r="D90">
-        <v>1987</v>
       </c>
       <c r="E90" t="s">
         <v>11</v>
@@ -4970,9 +4982,6 @@
       <c r="B91" t="s">
         <v>321</v>
       </c>
-      <c r="D91">
-        <v>1991</v>
-      </c>
       <c r="E91" t="s">
         <v>11</v>
       </c>
@@ -4981,14 +4990,14 @@
       </c>
     </row>
     <row r="92" spans="2:6">
-      <c r="B92" t="s">
+      <c r="B92" s="3" t="s">
         <v>322</v>
       </c>
       <c r="C92" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="D92">
-        <v>1984</v>
+        <v>1987</v>
       </c>
       <c r="E92" t="s">
         <v>11</v>
@@ -5001,11 +5010,8 @@
       <c r="B93" t="s">
         <v>323</v>
       </c>
-      <c r="C93" t="s">
-        <v>324</v>
-      </c>
       <c r="D93">
-        <v>1993</v>
+        <v>1991</v>
       </c>
       <c r="E93" t="s">
         <v>11</v>
@@ -5016,13 +5022,13 @@
     </row>
     <row r="94" spans="2:6">
       <c r="B94" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C94" t="s">
-        <v>326</v>
+        <v>229</v>
       </c>
       <c r="D94">
-        <v>1989</v>
+        <v>1984</v>
       </c>
       <c r="E94" t="s">
         <v>11</v>
@@ -5033,13 +5039,13 @@
     </row>
     <row r="95" spans="2:6">
       <c r="B95" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C95" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D95">
-        <v>1986</v>
+        <v>1993</v>
       </c>
       <c r="E95" t="s">
         <v>11</v>
@@ -5050,13 +5056,13 @@
     </row>
     <row r="96" spans="2:6">
       <c r="B96" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C96" t="s">
-        <v>223</v>
+        <v>328</v>
       </c>
       <c r="D96">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="E96" t="s">
         <v>11</v>
@@ -5067,13 +5073,13 @@
     </row>
     <row r="97" spans="2:6">
       <c r="B97" t="s">
+        <v>329</v>
+      </c>
+      <c r="C97" t="s">
         <v>330</v>
       </c>
-      <c r="C97" t="s">
-        <v>229</v>
-      </c>
       <c r="D97">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="E97" t="s">
         <v>11</v>
@@ -5087,10 +5093,10 @@
         <v>331</v>
       </c>
       <c r="C98" t="s">
-        <v>328</v>
+        <v>223</v>
       </c>
       <c r="D98">
-        <v>1990</v>
+        <v>1988</v>
       </c>
       <c r="E98" t="s">
         <v>11</v>
@@ -5121,10 +5127,10 @@
         <v>333</v>
       </c>
       <c r="C100" t="s">
-        <v>324</v>
+        <v>330</v>
       </c>
       <c r="D100">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="E100" t="s">
         <v>11</v>
@@ -5135,13 +5141,13 @@
     </row>
     <row r="101" spans="2:6">
       <c r="B101" t="s">
-        <v>200</v>
+        <v>334</v>
       </c>
       <c r="C101" t="s">
-        <v>334</v>
+        <v>229</v>
       </c>
       <c r="D101">
-        <v>1980</v>
+        <v>1985</v>
       </c>
       <c r="E101" t="s">
         <v>11</v>
@@ -5152,13 +5158,13 @@
     </row>
     <row r="102" spans="2:6">
       <c r="B102" t="s">
-        <v>148</v>
+        <v>335</v>
       </c>
       <c r="C102" t="s">
-        <v>251</v>
+        <v>326</v>
       </c>
       <c r="D102">
-        <v>1988</v>
+        <v>1991</v>
       </c>
       <c r="E102" t="s">
         <v>11</v>
@@ -5169,13 +5175,13 @@
     </row>
     <row r="103" spans="2:6">
       <c r="B103" t="s">
-        <v>335</v>
+        <v>200</v>
       </c>
       <c r="C103" t="s">
         <v>336</v>
       </c>
       <c r="D103">
-        <v>1990</v>
+        <v>1980</v>
       </c>
       <c r="E103" t="s">
         <v>11</v>
@@ -5186,13 +5192,13 @@
     </row>
     <row r="104" spans="2:6">
       <c r="B104" t="s">
-        <v>337</v>
+        <v>148</v>
       </c>
       <c r="C104" t="s">
-        <v>73</v>
+        <v>253</v>
       </c>
       <c r="D104">
-        <v>1982</v>
+        <v>1988</v>
       </c>
       <c r="E104" t="s">
         <v>11</v>
@@ -5203,13 +5209,13 @@
     </row>
     <row r="105" spans="2:6">
       <c r="B105" t="s">
-        <v>219</v>
+        <v>337</v>
       </c>
       <c r="C105" t="s">
-        <v>223</v>
+        <v>338</v>
       </c>
       <c r="D105">
-        <v>1987</v>
+        <v>1990</v>
       </c>
       <c r="E105" t="s">
         <v>11</v>
@@ -5220,13 +5226,13 @@
     </row>
     <row r="106" spans="2:6">
       <c r="B106" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C106" t="s">
-        <v>339</v>
+        <v>73</v>
       </c>
       <c r="D106">
-        <v>1985</v>
+        <v>1982</v>
       </c>
       <c r="E106" t="s">
         <v>11</v>
@@ -5237,10 +5243,10 @@
     </row>
     <row r="107" spans="2:6">
       <c r="B107" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="C107" t="s">
-        <v>340</v>
+        <v>223</v>
       </c>
       <c r="D107">
         <v>1987</v>
@@ -5254,13 +5260,13 @@
     </row>
     <row r="108" spans="2:6">
       <c r="B108" t="s">
+        <v>340</v>
+      </c>
+      <c r="C108" t="s">
         <v>341</v>
       </c>
-      <c r="C108" t="s">
-        <v>328</v>
-      </c>
       <c r="D108">
-        <v>1988</v>
+        <v>1985</v>
       </c>
       <c r="E108" t="s">
         <v>11</v>
@@ -5271,13 +5277,13 @@
     </row>
     <row r="109" spans="2:6">
       <c r="B109" t="s">
+        <v>189</v>
+      </c>
+      <c r="C109" t="s">
         <v>342</v>
       </c>
-      <c r="C109" t="s">
-        <v>229</v>
-      </c>
       <c r="D109">
-        <v>1992</v>
+        <v>1987</v>
       </c>
       <c r="E109" t="s">
         <v>11</v>
@@ -5291,10 +5297,10 @@
         <v>343</v>
       </c>
       <c r="C110" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D110">
-        <v>1985</v>
+        <v>1988</v>
       </c>
       <c r="E110" t="s">
         <v>11</v>
@@ -5308,10 +5314,10 @@
         <v>344</v>
       </c>
       <c r="C111" t="s">
-        <v>62</v>
+        <v>229</v>
       </c>
       <c r="D111">
-        <v>1987</v>
+        <v>1992</v>
       </c>
       <c r="E111" t="s">
         <v>11</v>
@@ -5325,10 +5331,10 @@
         <v>345</v>
       </c>
       <c r="C112" t="s">
-        <v>229</v>
+        <v>330</v>
       </c>
       <c r="D112">
-        <v>1992</v>
+        <v>1985</v>
       </c>
       <c r="E112" t="s">
         <v>11</v>
@@ -5339,13 +5345,13 @@
     </row>
     <row r="113" spans="2:6">
       <c r="B113" t="s">
-        <v>186</v>
+        <v>346</v>
       </c>
       <c r="C113" t="s">
-        <v>229</v>
+        <v>62</v>
       </c>
       <c r="D113">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="E113" t="s">
         <v>11</v>
@@ -5356,13 +5362,13 @@
     </row>
     <row r="114" spans="2:6">
       <c r="B114" t="s">
-        <v>145</v>
+        <v>347</v>
       </c>
       <c r="C114" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="D114">
-        <v>1988</v>
+        <v>1992</v>
       </c>
       <c r="E114" t="s">
         <v>11</v>
@@ -5373,13 +5379,13 @@
     </row>
     <row r="115" spans="2:6">
       <c r="B115" t="s">
-        <v>346</v>
+        <v>186</v>
       </c>
       <c r="C115" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="D115">
-        <v>1985</v>
+        <v>1988</v>
       </c>
       <c r="E115" t="s">
         <v>11</v>
@@ -5390,13 +5396,13 @@
     </row>
     <row r="116" spans="2:6">
       <c r="B116" t="s">
-        <v>347</v>
+        <v>145</v>
       </c>
       <c r="C116" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D116">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="E116" t="s">
         <v>11</v>
@@ -5410,10 +5416,10 @@
         <v>348</v>
       </c>
       <c r="C117" t="s">
-        <v>349</v>
+        <v>253</v>
       </c>
       <c r="D117">
-        <v>1991</v>
+        <v>1985</v>
       </c>
       <c r="E117" t="s">
         <v>11</v>
@@ -5424,13 +5430,13 @@
     </row>
     <row r="118" spans="2:6">
       <c r="B118" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C118" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="D118">
-        <v>1990</v>
+        <v>1987</v>
       </c>
       <c r="E118" t="s">
         <v>11</v>
@@ -5441,13 +5447,13 @@
     </row>
     <row r="119" spans="2:6">
       <c r="B119" t="s">
+        <v>350</v>
+      </c>
+      <c r="C119" t="s">
         <v>351</v>
       </c>
-      <c r="C119" t="s">
-        <v>127</v>
-      </c>
       <c r="D119">
-        <v>1988</v>
+        <v>1991</v>
       </c>
       <c r="E119" t="s">
         <v>11</v>
@@ -5461,10 +5467,10 @@
         <v>352</v>
       </c>
       <c r="C120" t="s">
-        <v>353</v>
+        <v>229</v>
       </c>
       <c r="D120">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="E120" t="s">
         <v>11</v>
@@ -5475,13 +5481,13 @@
     </row>
     <row r="121" spans="2:6">
       <c r="B121" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C121" t="s">
-        <v>251</v>
+        <v>127</v>
       </c>
       <c r="D121">
-        <v>1991</v>
+        <v>1988</v>
       </c>
       <c r="E121" t="s">
         <v>11</v>
@@ -5492,13 +5498,13 @@
     </row>
     <row r="122" spans="2:6">
       <c r="B122" t="s">
+        <v>354</v>
+      </c>
+      <c r="C122" t="s">
         <v>355</v>
       </c>
-      <c r="C122" t="s">
-        <v>73</v>
-      </c>
       <c r="D122">
-        <v>1983</v>
+        <v>1989</v>
       </c>
       <c r="E122" t="s">
         <v>11</v>
@@ -5509,13 +5515,13 @@
     </row>
     <row r="123" spans="2:6">
       <c r="B123" t="s">
-        <v>150</v>
+        <v>356</v>
       </c>
       <c r="C123" t="s">
-        <v>65</v>
+        <v>253</v>
       </c>
       <c r="D123">
-        <v>1987</v>
+        <v>1991</v>
       </c>
       <c r="E123" t="s">
         <v>11</v>
@@ -5526,13 +5532,13 @@
     </row>
     <row r="124" spans="2:6">
       <c r="B124" t="s">
-        <v>187</v>
+        <v>357</v>
       </c>
       <c r="C124" t="s">
-        <v>251</v>
+        <v>73</v>
       </c>
       <c r="D124">
-        <v>2003</v>
+        <v>1983</v>
       </c>
       <c r="E124" t="s">
         <v>11</v>
@@ -5543,13 +5549,13 @@
     </row>
     <row r="125" spans="2:6">
       <c r="B125" t="s">
-        <v>356</v>
+        <v>150</v>
       </c>
       <c r="C125" t="s">
-        <v>251</v>
+        <v>65</v>
       </c>
       <c r="D125">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="E125" t="s">
         <v>11</v>
@@ -5560,7 +5566,13 @@
     </row>
     <row r="126" spans="2:6">
       <c r="B126" t="s">
-        <v>357</v>
+        <v>187</v>
+      </c>
+      <c r="C126" t="s">
+        <v>253</v>
+      </c>
+      <c r="D126">
+        <v>2003</v>
       </c>
       <c r="E126" t="s">
         <v>11</v>
@@ -5574,10 +5586,10 @@
         <v>358</v>
       </c>
       <c r="C127" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="D127">
-        <v>1991</v>
+        <v>1986</v>
       </c>
       <c r="E127" t="s">
         <v>11</v>
@@ -5590,12 +5602,6 @@
       <c r="B128" t="s">
         <v>359</v>
       </c>
-      <c r="C128" t="s">
-        <v>251</v>
-      </c>
-      <c r="D128">
-        <v>1985</v>
-      </c>
       <c r="E128" t="s">
         <v>11</v>
       </c>
@@ -5608,7 +5614,7 @@
         <v>360</v>
       </c>
       <c r="C129" t="s">
-        <v>361</v>
+        <v>229</v>
       </c>
       <c r="D129">
         <v>1991</v>
@@ -5622,13 +5628,13 @@
     </row>
     <row r="130" spans="2:6">
       <c r="B130" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C130" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D130">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="E130" t="s">
         <v>11</v>
@@ -5639,10 +5645,10 @@
     </row>
     <row r="131" spans="2:6">
       <c r="B131" t="s">
+        <v>362</v>
+      </c>
+      <c r="C131" t="s">
         <v>363</v>
-      </c>
-      <c r="C131" t="s">
-        <v>251</v>
       </c>
       <c r="D131">
         <v>1991</v>
@@ -5659,10 +5665,10 @@
         <v>364</v>
       </c>
       <c r="C132" t="s">
-        <v>365</v>
+        <v>253</v>
       </c>
       <c r="D132">
-        <v>1984</v>
+        <v>1986</v>
       </c>
       <c r="E132" t="s">
         <v>11</v>
@@ -5673,7 +5679,13 @@
     </row>
     <row r="133" spans="2:6">
       <c r="B133" t="s">
-        <v>366</v>
+        <v>365</v>
+      </c>
+      <c r="C133" t="s">
+        <v>253</v>
+      </c>
+      <c r="D133">
+        <v>1991</v>
       </c>
       <c r="E133" t="s">
         <v>11</v>
@@ -5684,13 +5696,13 @@
     </row>
     <row r="134" spans="2:6">
       <c r="B134" t="s">
+        <v>366</v>
+      </c>
+      <c r="C134" t="s">
         <v>367</v>
       </c>
-      <c r="C134" t="s">
-        <v>251</v>
-      </c>
       <c r="D134">
-        <v>1990</v>
+        <v>1984</v>
       </c>
       <c r="E134" t="s">
         <v>11</v>
@@ -5703,12 +5715,6 @@
       <c r="B135" t="s">
         <v>368</v>
       </c>
-      <c r="C135" t="s">
-        <v>251</v>
-      </c>
-      <c r="D135">
-        <v>1990</v>
-      </c>
       <c r="E135" t="s">
         <v>11</v>
       </c>
@@ -5721,10 +5727,10 @@
         <v>369</v>
       </c>
       <c r="C136" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D136">
-        <v>1992</v>
+        <v>1990</v>
       </c>
       <c r="E136" t="s">
         <v>11</v>
@@ -5738,10 +5744,10 @@
         <v>370</v>
       </c>
       <c r="C137" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D137">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="E137" t="s">
         <v>11</v>
@@ -5755,10 +5761,10 @@
         <v>371</v>
       </c>
       <c r="C138" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D138">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="E138" t="s">
         <v>11</v>
@@ -5772,10 +5778,10 @@
         <v>372</v>
       </c>
       <c r="C139" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="D139">
-        <v>1993</v>
+        <v>1989</v>
       </c>
       <c r="E139" t="s">
         <v>11</v>
@@ -5786,10 +5792,13 @@
     </row>
     <row r="140" spans="2:6">
       <c r="B140" t="s">
-        <v>154</v>
+        <v>373</v>
       </c>
       <c r="C140" t="s">
-        <v>373</v>
+        <v>253</v>
+      </c>
+      <c r="D140">
+        <v>1993</v>
       </c>
       <c r="E140" t="s">
         <v>11</v>
@@ -5803,10 +5812,10 @@
         <v>374</v>
       </c>
       <c r="C141" t="s">
-        <v>251</v>
+        <v>229</v>
       </c>
       <c r="D141">
-        <v>1985</v>
+        <v>1993</v>
       </c>
       <c r="E141" t="s">
         <v>11</v>
@@ -5817,13 +5826,10 @@
     </row>
     <row r="142" spans="2:6">
       <c r="B142" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="C142" t="s">
-        <v>251</v>
-      </c>
-      <c r="D142">
-        <v>1987</v>
+        <v>375</v>
       </c>
       <c r="E142" t="s">
         <v>11</v>
@@ -5834,7 +5840,13 @@
     </row>
     <row r="143" spans="2:6">
       <c r="B143" t="s">
-        <v>375</v>
+        <v>376</v>
+      </c>
+      <c r="C143" t="s">
+        <v>253</v>
+      </c>
+      <c r="D143">
+        <v>1985</v>
       </c>
       <c r="E143" t="s">
         <v>11</v>
@@ -5845,7 +5857,13 @@
     </row>
     <row r="144" spans="2:6">
       <c r="B144" t="s">
-        <v>376</v>
+        <v>188</v>
+      </c>
+      <c r="C144" t="s">
+        <v>253</v>
+      </c>
+      <c r="D144">
+        <v>1987</v>
       </c>
       <c r="E144" t="s">
         <v>11</v>
@@ -5856,13 +5874,7 @@
     </row>
     <row r="145" spans="2:6">
       <c r="B145" t="s">
-        <v>156</v>
-      </c>
-      <c r="C145" t="s">
-        <v>353</v>
-      </c>
-      <c r="D145">
-        <v>1991</v>
+        <v>377</v>
       </c>
       <c r="E145" t="s">
         <v>11</v>
@@ -5873,13 +5885,7 @@
     </row>
     <row r="146" spans="2:6">
       <c r="B146" t="s">
-        <v>157</v>
-      </c>
-      <c r="C146" t="s">
-        <v>62</v>
-      </c>
-      <c r="D146">
-        <v>1989</v>
+        <v>378</v>
       </c>
       <c r="E146" t="s">
         <v>11</v>
@@ -5890,13 +5896,13 @@
     </row>
     <row r="147" spans="2:6">
       <c r="B147" t="s">
-        <v>377</v>
+        <v>156</v>
       </c>
       <c r="C147" t="s">
-        <v>378</v>
+        <v>355</v>
       </c>
       <c r="D147">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="E147" t="s">
         <v>11</v>
@@ -5907,13 +5913,13 @@
     </row>
     <row r="148" spans="2:6">
       <c r="B148" t="s">
-        <v>379</v>
+        <v>157</v>
       </c>
       <c r="C148" t="s">
-        <v>251</v>
+        <v>62</v>
       </c>
       <c r="D148">
-        <v>1991</v>
+        <v>1989</v>
       </c>
       <c r="E148" t="s">
         <v>11</v>
@@ -5924,13 +5930,13 @@
     </row>
     <row r="149" spans="2:6">
       <c r="B149" t="s">
+        <v>379</v>
+      </c>
+      <c r="C149" t="s">
         <v>380</v>
       </c>
-      <c r="C149" t="s">
-        <v>381</v>
-      </c>
       <c r="D149">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="E149" t="s">
         <v>11</v>
@@ -5941,7 +5947,13 @@
     </row>
     <row r="150" spans="2:6">
       <c r="B150" t="s">
-        <v>382</v>
+        <v>381</v>
+      </c>
+      <c r="C150" t="s">
+        <v>253</v>
+      </c>
+      <c r="D150">
+        <v>1991</v>
       </c>
       <c r="E150" t="s">
         <v>11</v>
@@ -5952,13 +5964,13 @@
     </row>
     <row r="151" spans="2:6">
       <c r="B151" t="s">
+        <v>382</v>
+      </c>
+      <c r="C151" t="s">
         <v>383</v>
       </c>
-      <c r="C151" t="s">
-        <v>251</v>
-      </c>
       <c r="D151">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="E151" t="s">
         <v>11</v>
@@ -5971,12 +5983,6 @@
       <c r="B152" t="s">
         <v>384</v>
       </c>
-      <c r="C152" t="s">
-        <v>73</v>
-      </c>
-      <c r="D152">
-        <v>1984</v>
-      </c>
       <c r="E152" t="s">
         <v>11</v>
       </c>
@@ -5989,10 +5995,10 @@
         <v>385</v>
       </c>
       <c r="C153" t="s">
-        <v>353</v>
+        <v>253</v>
       </c>
       <c r="D153">
-        <v>1986</v>
+        <v>1990</v>
       </c>
       <c r="E153" t="s">
         <v>11</v>
@@ -6006,7 +6012,7 @@
         <v>386</v>
       </c>
       <c r="C154" t="s">
-        <v>229</v>
+        <v>73</v>
       </c>
       <c r="D154">
         <v>1984</v>
@@ -6020,10 +6026,13 @@
     </row>
     <row r="155" spans="2:6">
       <c r="B155" t="s">
-        <v>193</v>
+        <v>387</v>
+      </c>
+      <c r="C155" t="s">
+        <v>355</v>
       </c>
       <c r="D155">
-        <v>1990</v>
+        <v>1986</v>
       </c>
       <c r="E155" t="s">
         <v>11</v>
@@ -6034,10 +6043,13 @@
     </row>
     <row r="156" spans="2:6">
       <c r="B156" t="s">
-        <v>387</v>
+        <v>388</v>
+      </c>
+      <c r="C156" t="s">
+        <v>229</v>
       </c>
       <c r="D156">
-        <v>1991</v>
+        <v>1984</v>
       </c>
       <c r="E156" t="s">
         <v>11</v>
@@ -6048,13 +6060,10 @@
     </row>
     <row r="157" spans="2:6">
       <c r="B157" t="s">
-        <v>216</v>
-      </c>
-      <c r="C157" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="D157">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="E157" t="s">
         <v>11</v>
@@ -6065,7 +6074,10 @@
     </row>
     <row r="158" spans="2:6">
       <c r="B158" t="s">
-        <v>388</v>
+        <v>389</v>
+      </c>
+      <c r="D158">
+        <v>1991</v>
       </c>
       <c r="E158" t="s">
         <v>11</v>
@@ -6076,13 +6088,13 @@
     </row>
     <row r="159" spans="2:6">
       <c r="B159" t="s">
-        <v>159</v>
+        <v>216</v>
       </c>
       <c r="C159" t="s">
-        <v>336</v>
+        <v>223</v>
       </c>
       <c r="D159">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="E159" t="s">
         <v>11</v>
@@ -6093,13 +6105,7 @@
     </row>
     <row r="160" spans="2:6">
       <c r="B160" t="s">
-        <v>389</v>
-      </c>
-      <c r="C160" t="s">
         <v>390</v>
-      </c>
-      <c r="D160">
-        <v>2008</v>
       </c>
       <c r="E160" t="s">
         <v>11</v>
@@ -6110,13 +6116,13 @@
     </row>
     <row r="161" spans="2:6">
       <c r="B161" t="s">
-        <v>391</v>
+        <v>159</v>
       </c>
       <c r="C161" t="s">
-        <v>392</v>
+        <v>338</v>
       </c>
       <c r="D161">
-        <v>2008</v>
+        <v>1990</v>
       </c>
       <c r="E161" t="s">
         <v>11</v>
@@ -6127,13 +6133,13 @@
     </row>
     <row r="162" spans="2:6">
       <c r="B162" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C162" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D162">
-        <v>1982</v>
+        <v>2008</v>
       </c>
       <c r="E162" t="s">
         <v>11</v>
@@ -6144,10 +6150,10 @@
     </row>
     <row r="163" spans="2:6">
       <c r="B163" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C163" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="D163">
         <v>2008</v>
@@ -6161,13 +6167,13 @@
     </row>
     <row r="164" spans="2:6">
       <c r="B164" t="s">
+        <v>395</v>
+      </c>
+      <c r="C164" t="s">
         <v>396</v>
       </c>
-      <c r="C164" t="s">
-        <v>73</v>
-      </c>
       <c r="D164">
-        <v>1980</v>
+        <v>1982</v>
       </c>
       <c r="E164" t="s">
         <v>11</v>
@@ -6181,7 +6187,10 @@
         <v>397</v>
       </c>
       <c r="C165" t="s">
-        <v>398</v>
+        <v>392</v>
+      </c>
+      <c r="D165">
+        <v>2008</v>
       </c>
       <c r="E165" t="s">
         <v>11</v>
@@ -6192,13 +6201,13 @@
     </row>
     <row r="166" spans="2:6">
       <c r="B166" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C166" t="s">
-        <v>400</v>
+        <v>73</v>
       </c>
       <c r="D166">
-        <v>2009</v>
+        <v>1980</v>
       </c>
       <c r="E166" t="s">
         <v>11</v>
@@ -6209,13 +6218,10 @@
     </row>
     <row r="167" spans="2:6">
       <c r="B167" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="C167" t="s">
-        <v>402</v>
-      </c>
-      <c r="D167">
-        <v>1990</v>
+        <v>400</v>
       </c>
       <c r="E167" t="s">
         <v>11</v>
@@ -6226,13 +6232,13 @@
     </row>
     <row r="168" spans="2:6">
       <c r="B168" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C168" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D168">
-        <v>1992</v>
+        <v>2009</v>
       </c>
       <c r="E168" t="s">
         <v>11</v>
@@ -6243,10 +6249,13 @@
     </row>
     <row r="169" spans="2:6">
       <c r="B169" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C169" t="s">
-        <v>406</v>
+        <v>404</v>
+      </c>
+      <c r="D169">
+        <v>1990</v>
       </c>
       <c r="E169" t="s">
         <v>11</v>
@@ -6257,13 +6266,13 @@
     </row>
     <row r="170" spans="2:6">
       <c r="B170" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C170" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D170">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="E170" t="s">
         <v>11</v>
@@ -6274,7 +6283,10 @@
     </row>
     <row r="171" spans="2:6">
       <c r="B171" t="s">
-        <v>409</v>
+        <v>407</v>
+      </c>
+      <c r="C171" t="s">
+        <v>408</v>
       </c>
       <c r="E171" t="s">
         <v>11</v>
@@ -6285,7 +6297,13 @@
     </row>
     <row r="172" spans="2:6">
       <c r="B172" t="s">
+        <v>409</v>
+      </c>
+      <c r="C172" t="s">
         <v>410</v>
+      </c>
+      <c r="D172">
+        <v>1993</v>
       </c>
       <c r="E172" t="s">
         <v>11</v>
@@ -6419,12 +6437,6 @@
       <c r="B184" t="s">
         <v>422</v>
       </c>
-      <c r="C184" t="s">
-        <v>423</v>
-      </c>
-      <c r="D184">
-        <v>1988</v>
-      </c>
       <c r="E184" t="s">
         <v>11</v>
       </c>
@@ -6434,13 +6446,7 @@
     </row>
     <row r="185" spans="2:6">
       <c r="B185" t="s">
-        <v>424</v>
-      </c>
-      <c r="C185" t="s">
-        <v>326</v>
-      </c>
-      <c r="D185">
-        <v>1988</v>
+        <v>423</v>
       </c>
       <c r="E185" t="s">
         <v>11</v>
@@ -6451,7 +6457,13 @@
     </row>
     <row r="186" spans="2:6">
       <c r="B186" t="s">
+        <v>424</v>
+      </c>
+      <c r="C186" t="s">
         <v>425</v>
+      </c>
+      <c r="D186">
+        <v>1988</v>
       </c>
       <c r="E186" t="s">
         <v>11</v>
@@ -6464,6 +6476,12 @@
       <c r="B187" t="s">
         <v>426</v>
       </c>
+      <c r="C187" t="s">
+        <v>328</v>
+      </c>
+      <c r="D187">
+        <v>1988</v>
+      </c>
       <c r="E187" t="s">
         <v>11</v>
       </c>
@@ -6482,7 +6500,10 @@
         <v>112</v>
       </c>
     </row>
-    <row r="189" spans="5:6">
+    <row r="189" spans="2:6">
+      <c r="B189" t="s">
+        <v>428</v>
+      </c>
       <c r="E189" t="s">
         <v>11</v>
       </c>
@@ -6490,7 +6511,10 @@
         <v>112</v>
       </c>
     </row>
-    <row r="190" spans="5:6">
+    <row r="190" spans="2:6">
+      <c r="B190" t="s">
+        <v>429</v>
+      </c>
       <c r="E190" t="s">
         <v>11</v>
       </c>
@@ -6799,6 +6823,22 @@
         <v>11</v>
       </c>
       <c r="F228" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="229" spans="5:6">
+      <c r="E229" t="s">
+        <v>11</v>
+      </c>
+      <c r="F229" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="230" spans="5:6">
+      <c r="E230" t="s">
+        <v>11</v>
+      </c>
+      <c r="F230" t="s">
         <v>112</v>
       </c>
     </row>
@@ -6844,7 +6884,7 @@
     </row>
     <row r="2" spans="2:6">
       <c r="B2" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C2" t="s">
         <v>65</v>
@@ -6856,7 +6896,7 @@
         <v>69</v>
       </c>
       <c r="F2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="2:6">
@@ -6864,7 +6904,7 @@
         <v>126</v>
       </c>
       <c r="F3" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>